<commit_message>
Variant, Locations and Stock ready
</commit_message>
<xml_diff>
--- a/spec/fixtures/imported.xlsx
+++ b/spec/fixtures/imported.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" state="visible" r:id="rId2"/>
@@ -195,13 +195,13 @@
     <t xml:space="preserve">Región Metropolitana</t>
   </si>
   <si>
+    <t xml:space="preserve">Ubicación (Nom. Interno)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID Variante</t>
   </si>
   <si>
     <t xml:space="preserve">Cantidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID Ubicación</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -333,7 +333,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="7.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.72"/>
@@ -580,7 +580,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -671,115 +671,108 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="21.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="9.45"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="F2" s="1" t="n">
+        <v>12345</v>
+      </c>
       <c r="G2" s="1" t="n">
-        <v>12345</v>
-      </c>
-      <c r="H2" s="1" t="n">
         <v>76543469</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -802,19 +795,20 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.45"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -831,18 +825,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="D2" s="1" t="n">
         <v>20</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Categories (taxonomies) added to import
</commit_message>
<xml_diff>
--- a/spec/fixtures/imported.xlsx
+++ b/spec/fixtures/imported.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" state="visible" r:id="rId2"/>
@@ -90,7 +90,7 @@
     <t xml:space="preserve">Sí</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO</t>
+    <t xml:space="preserve">riri-&gt;ruru-&gt;rere, coco</t>
   </si>
   <si>
     <t xml:space="preserve">Por defecto</t>
@@ -320,8 +320,8 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -428,7 +428,7 @@
       <c r="M2" s="2" t="n">
         <v>43075</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -673,7 +673,7 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
No need for two excels
</commit_message>
<xml_diff>
--- a/spec/fixtures/imported.xlsx
+++ b/spec/fixtures/imported.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t xml:space="preserve">en molde de cupcake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
   </si>
   <si>
     <t xml:space="preserve">queque-en-molde-de-cupcake</t>
@@ -321,7 +318,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -330,7 +327,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="7.01"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="7.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.88"/>
@@ -401,38 +399,38 @@
       <c r="D2" s="1" t="n">
         <v>1500</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1" t="n">
+        <v>87654321</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>43075</v>
       </c>
       <c r="N2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -467,13 +465,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,10 +479,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,10 +490,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -530,13 +528,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,10 +542,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,10 +553,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -602,16 +600,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -634,7 +632,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>12345678</v>
@@ -699,57 +697,57 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>12345</v>
@@ -758,22 +756,22 @@
         <v>76543469</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -810,19 +808,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2</v>
@@ -839,7 +837,7 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Returns error for format and missing requires
</commit_message>
<xml_diff>
--- a/spec/fixtures/imported.xlsx
+++ b/spec/fixtures/imported.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t xml:space="preserve">ID*</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">Por defecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">queque2</t>
   </si>
   <si>
     <t xml:space="preserve">ID Producto*</t>
@@ -324,12 +327,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,7 +473,48 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>43075</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1470,23 +1514,23 @@
     <row r="1000" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="5">
+    <dataValidation allowBlank="true" operator="between" prompt="El ID debe ser único" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="A1:A2" type="custom">
+      <formula1>COUNTIF($A:$A,"="&amp;A1)  &lt; 2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" prompt="El SKU ya existe (en Productos o Variantes). Debe ser único." showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="E1:E2" type="custom">
       <formula1>AND(COUNTIF(Productos!$E:$E,"="&amp;Productos!E1)  &lt; 2, COUNTIF(Variantes!$D:$D,"="&amp;Productos!E1)  &lt; 1)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="El ID debe ser único" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="A1:A2" type="custom">
-      <formula1>COUNTIF($A:$A,"="&amp;A1)  &lt; 2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Se deben ingresar solo números" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="D2" type="custom">
+    <dataValidation allowBlank="true" operator="between" prompt="Se deben ingresar solo números" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="D2:D3" type="custom">
       <formula1>regexmatch(to_text(D2),"^[0-9]*$")=1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Debe ser Sí o No" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="between" prompt="Debe ser Sí o No" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L3" type="list">
       <formula1>"Sí,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Deber ingresar las categorías de la forma: riri-&gt;ruru-&gt;rere, coco" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="N2" type="custom">
+    <dataValidation allowBlank="true" operator="between" prompt="Deber ingresar las categorías de la forma: riri-&gt;ruru-&gt;rere, coco" showDropDown="true" showErrorMessage="true" showInputMessage="true" sqref="N2:N3" type="custom">
       <formula1>regexmatch(N2,"^((([A-z0-9]+-&gt;)*[A-z0-9]+)(, )?)*(([A-z0-9]+-&gt;)*[A-z0-9]+)?$")=1</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1508,10 +1552,10 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="1" sqref="A3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1535,16 +1579,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1584,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>12345678</v>
@@ -2659,7 +2703,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="A3 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2674,13 +2718,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -2711,7 +2755,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>19</v>
@@ -2745,10 +2789,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -3798,7 +3842,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3813,13 +3857,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3850,10 +3894,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -3884,10 +3928,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4937,7 +4981,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4965,40 +5009,40 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -5016,19 +5060,19 @@
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>12345</v>
@@ -5037,16 +5081,16 @@
         <v>76543469</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>19</v>
@@ -6097,7 +6141,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6114,19 +6158,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -6155,7 +6199,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
Fix Stock no variant import
</commit_message>
<xml_diff>
--- a/spec/fixtures/imported.xlsx
+++ b/spec/fixtures/imported.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t xml:space="preserve">ID*</t>
   </si>
@@ -206,6 +206,9 @@
   <si>
     <t xml:space="preserve">Cantidad*</t>
   </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
 </sst>
 </file>
 
@@ -329,7 +332,7 @@
   </sheetPr>
   <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -1555,7 +1558,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="1" sqref="A3 E1"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2703,7 +2706,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="A3 B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3842,7 +3845,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4981,7 +4984,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6136,12 +6139,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="A3 B3"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6232,7 +6235,20 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>